<commit_message>
After changes it works
</commit_message>
<xml_diff>
--- a/src/main/resources/Results.xlsx
+++ b/src/main/resources/Results.xlsx
@@ -6,13 +6,13 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Результаты ТОП 10" r:id="rId3" sheetId="1"/>
+    <sheet name="Результаты ТОП-10" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>№</t>
   </si>
@@ -23,28 +23,28 @@
     <t>Количество баллов</t>
   </si>
   <si>
+    <t>Смельчак</t>
+  </si>
+  <si>
     <t>Нюша хрюша</t>
   </si>
   <si>
-    <t>Вуди Вудпекер</t>
+    <t>Отвинта</t>
+  </si>
+  <si>
+    <t>Копатыч</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>Винни</t>
   </si>
   <si>
-    <t>Бегемоты в болоте</t>
-  </si>
-  <si>
     <t>Совунья</t>
   </si>
   <si>
     <t>Крош</t>
-  </si>
-  <si>
-    <t>Копатыч</t>
-  </si>
-  <si>
-    <t>Дим Димыч</t>
   </si>
 </sst>
 </file>
@@ -89,7 +89,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -114,7 +114,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>2004.0</v>
+        <v>160.0</v>
       </c>
     </row>
     <row r="3">
@@ -125,7 +125,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="n" s="0">
-        <v>136.0</v>
+        <v>156.0</v>
       </c>
     </row>
     <row r="4">
@@ -136,7 +136,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="n" s="0">
-        <v>90.0</v>
+        <v>143.0</v>
       </c>
     </row>
     <row r="5">
@@ -147,7 +147,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n" s="0">
-        <v>66.0</v>
+        <v>136.0</v>
       </c>
     </row>
     <row r="6">
@@ -158,7 +158,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="n" s="0">
-        <v>34.0</v>
+        <v>112.0</v>
       </c>
     </row>
     <row r="7">
@@ -169,7 +169,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="n" s="0">
-        <v>12.0</v>
+        <v>90.0</v>
       </c>
     </row>
     <row r="8">
@@ -180,7 +180,7 @@
         <v>9</v>
       </c>
       <c r="C8" t="n" s="0">
-        <v>5.0</v>
+        <v>66.0</v>
       </c>
     </row>
     <row r="9">
@@ -191,6 +191,17 @@
         <v>10</v>
       </c>
       <c r="C9" t="n" s="0">
+        <v>34.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n" s="0">
+        <v>9.0</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C10" t="n" s="0">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>